<commit_message>
[Test] Set first day 2026-01-09
</commit_message>
<xml_diff>
--- a/public/gifts_first.xlsx
+++ b/public/gifts_first.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wenliao\AMC_app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47284CAB-E64F-42B8-8824-A68BF2374629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49B906A-C687-44AD-8B51-BE470743ADCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="915" windowWidth="21795" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -372,7 +372,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -406,7 +406,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>